<commit_message>
Alterado a formataÃÃo da tabela
*Agora irÃ¡ aparecer o nome da matriz de comparaÃÃo de critÃrios na
tabela
*Cores alteradas para o erro, agora se o erro for maior que 5%(teste o
certo Ã©10) serÃ¡alterado a cor de fundo para vermelho, se nÃo verde.
</commit_message>
<xml_diff>
--- a/banco_de_dados/BD1.xlsx
+++ b/banco_de_dados/BD1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Smart\Documents\AHP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Smart\Documents\AHP\banco_de_dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -17,7 +17,7 @@
     <sheet name="PS" sheetId="3" r:id="rId3"/>
     <sheet name="RV" sheetId="4" r:id="rId4"/>
     <sheet name="MA" sheetId="5" r:id="rId5"/>
-    <sheet name="FP" sheetId="6" r:id="rId6"/>
+    <sheet name="Comprar um carro" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,10 +26,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>